<commit_message>
Corrected name of model variable "DB_Pforest"
</commit_message>
<xml_diff>
--- a/site_DATAexplore/FinalModelVariables_9.6.20.xlsx
+++ b/site_DATAexplore/FinalModelVariables_9.6.20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamjohnson/Desktop/Laura/Hallett_Lab/Repositories/thesis-mussels/site_DATAexplore/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073A14BE-E3A8-6343-8CB7-CEA680B2DF0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472BE41C-A567-F74F-8769-4DA81B982EFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="460" windowWidth="20340" windowHeight="16420" xr2:uid="{93482ABB-FAD0-E542-8695-4947CDE4C76D}"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="20340" windowHeight="16080" xr2:uid="{93482ABB-FAD0-E542-8695-4947CDE4C76D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -239,9 +239,6 @@
     <t>COW02</t>
   </si>
   <si>
-    <t>DP_Pforest</t>
-  </si>
-  <si>
     <t>HUC_Pforest</t>
   </si>
   <si>
@@ -258,6 +255,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>DB_Pforest</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -651,22 +651,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
         <v>68</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>70</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>71</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>72</v>
-      </c>
-      <c r="I1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2029,7 +2029,7 @@
         <v>28.969769769999999</v>
       </c>
       <c r="I48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2058,7 +2058,7 @@
         <v>28.969769769999999</v>
       </c>
       <c r="I49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2087,7 +2087,7 @@
         <v>28.969769769999999</v>
       </c>
       <c r="I50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2116,7 +2116,7 @@
         <v>28.969769769999999</v>
       </c>
       <c r="I51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2145,7 +2145,7 @@
         <v>439.97000739999999</v>
       </c>
       <c r="I52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Not sure what the modification was on this...?
</commit_message>
<xml_diff>
--- a/site_DATAexplore/FinalModelVariables_9.6.20.xlsx
+++ b/site_DATAexplore/FinalModelVariables_9.6.20.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamjohnson/Desktop/Laura/Hallett_Lab/Repositories/thesis-mussels/site_DATAexplore/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472BE41C-A567-F74F-8769-4DA81B982EFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC02B86-9B68-A348-A732-A6A52B18496D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="20340" windowHeight="16080" xr2:uid="{93482ABB-FAD0-E542-8695-4947CDE4C76D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -632,7 +632,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>